<commit_message>
changes related to example sentencs
</commit_message>
<xml_diff>
--- a/1_sentiment/synthetic/input/sentiment_example_sentences.xlsx
+++ b/1_sentiment/synthetic/input/sentiment_example_sentences.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmerx/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8527fed3e781c182/COMP80004_PhDResearch/RESEARCH/PROJECTS/3_evaluation^Mvalidation - ACL 2025/ICL/1_sentiment/synthetic/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFA09121-BD05-4446-85A6-D85CA360F83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="8_{AFA09121-BD05-4446-85A6-D85CA360F83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94F11060-7A4A-4869-92F4-3240ECE03C9C}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="840" windowWidth="27640" windowHeight="16940" xr2:uid="{56DC9B05-F223-784B-BB17-0833FFAD395C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{56DC9B05-F223-784B-BB17-0833FFAD395C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="academic" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,25 +36,316 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
   <si>
     <t>baseline</t>
   </si>
   <si>
-    <t>positive sentiment</t>
-  </si>
-  <si>
-    <t>negative sentiment</t>
-  </si>
-  <si>
-    <t>In a 24-yr-old female patient with a 12-yr history of kleptomania, it appeared that the behavior was maintained because it reduced anxiety in relevant situations.</t>
+    <t>target</t>
+  </si>
+  <si>
+    <t>abuse</t>
+  </si>
+  <si>
+    <t>anxiety</t>
+  </si>
+  <si>
+    <t>depression</t>
+  </si>
+  <si>
+    <t>trauma</t>
+  </si>
+  <si>
+    <t>mental_health</t>
+  </si>
+  <si>
+    <t>The study documented instances of verbal abuse within familial relationships.</t>
+  </si>
+  <si>
+    <t>The study highlighted the resilience of individuals who overcame verbal abuse within familial relationships.</t>
+  </si>
+  <si>
+    <t>positive_sentiment</t>
+  </si>
+  <si>
+    <t>negative_sentiment</t>
+  </si>
+  <si>
+    <t>mental_illness</t>
+  </si>
+  <si>
+    <t>Research explored patterns of abuse among different socioeconomic groups.</t>
+  </si>
+  <si>
+    <t>Research emphasized the strength of communities that supported victims of abuse and facilitated recovery.</t>
+  </si>
+  <si>
+    <t>The prevalence of abuse was assessed across multiple cultural contexts.</t>
+  </si>
+  <si>
+    <t>The prevalence of abuse was mitigated by community interventions aimed at fostering resilience and healing.</t>
+  </si>
+  <si>
+    <t>The prevalence of abuse was associated with significant psychological and social dysfunction in affected populations.</t>
+  </si>
+  <si>
+    <t>Reports highlighted how abuse disrupts trust in personal relationships.</t>
+  </si>
+  <si>
+    <t>Reports celebrated the ability of survivors to rebuild trust and find support after abuse.</t>
+  </si>
+  <si>
+    <t>Reports underscored how abuse erodes trust and creates lasting relational difficulties.</t>
+  </si>
+  <si>
+    <t>The study investigated the association between abuse and psychological well-being.</t>
+  </si>
+  <si>
+    <t>The study highlighted improved well-being among survivors who accessed effective support after abuse.</t>
+  </si>
+  <si>
+    <t>The research examined factors contributing to anxiety in adolescents.</t>
+  </si>
+  <si>
+    <t>The research revealed how anxiety in adolescents led to social withdrawal and academic difficulties.</t>
+  </si>
+  <si>
+    <t>The study focused on anxiety symptoms in workplace environments.</t>
+  </si>
+  <si>
+    <t>The study emphasized the benefits of workplace programs that alleviated anxiety and improved employee well-being.</t>
+  </si>
+  <si>
+    <t>The study found that anxiety in workplace environments correlated with reduced productivity and increased stress levels.</t>
+  </si>
+  <si>
+    <t>The paper analyzed the prevalence of anxiety among university students.</t>
+  </si>
+  <si>
+    <t>The paper showcased effective coping mechanisms that reduced anxiety among university students.</t>
+  </si>
+  <si>
+    <t>The study reviewed anxiety in the context of social media use.</t>
+  </si>
+  <si>
+    <t>The study highlighted how mindfulness interventions reduced anxiety related to social media use.</t>
+  </si>
+  <si>
+    <t>The study revealed that excessive social media use exacerbated anxiety and feelings of inadequacy.</t>
+  </si>
+  <si>
+    <t>The research explored anxiety during major life transitions.</t>
+  </si>
+  <si>
+    <t>The research highlighted personal growth and resilience in individuals who managed anxiety during life transitions.</t>
+  </si>
+  <si>
+    <t>The research revealed the disruptive impact of anxiety during life transitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> including emotional distress and uncertainty.</t>
+  </si>
+  <si>
+    <t>The study investigated the relationship between social support and depression.</t>
+  </si>
+  <si>
+    <t>The study showed how increased social support reduced symptoms of depression and improved emotional well-being.</t>
+  </si>
+  <si>
+    <t>The study demonstrated how a lack of social support worsened symptoms of depression over time.</t>
+  </si>
+  <si>
+    <t>The research examined depression in older adults across different living arrangements.</t>
+  </si>
+  <si>
+    <t>The research highlighted how community engagement programs improved mood and reduced depression in older adults.</t>
+  </si>
+  <si>
+    <t>The research found that isolation in older adults was strongly associated with increased depression.</t>
+  </si>
+  <si>
+    <t>The paper reviewed cultural differences in the experience of depression.</t>
+  </si>
+  <si>
+    <t>The paper celebrated culturally sensitive interventions that improved outcomes for individuals with depression.</t>
+  </si>
+  <si>
+    <t>The study analyzed depression in caregivers of individuals with chronic illnesses.</t>
+  </si>
+  <si>
+    <t>The study highlighted how peer support groups helped caregivers manage depression and maintain emotional balance.</t>
+  </si>
+  <si>
+    <t>The study showed that depression in caregivers contributed to burnout and long-term health challenges.</t>
+  </si>
+  <si>
+    <t>The research explored depression in the aftermath of natural disasters.</t>
+  </si>
+  <si>
+    <t>The research highlighted the resilience of communities that recovered emotionally from depression caused by natural disasters.</t>
+  </si>
+  <si>
+    <t>The study investigated the impact of work-life balance on mental health.</t>
+  </si>
+  <si>
+    <t>The study highlighted the improvement in mental health when work-life balance programs were implemented.</t>
+  </si>
+  <si>
+    <t>The study revealed that poor work-life balance significantly deteriorated mental health in employees.</t>
+  </si>
+  <si>
+    <t>The paper explored the relationship between physical activity and mental health.</t>
+  </si>
+  <si>
+    <t>The paper demonstrated how regular physical activity enhanced mental health outcomes.</t>
+  </si>
+  <si>
+    <t>The paper revealed that a sedentary lifestyle negatively impacted mental health over time.</t>
+  </si>
+  <si>
+    <t>The research analyzed mental health trends in urban populations.</t>
+  </si>
+  <si>
+    <t>The research emphasized how urban planning initiatives improved mental health through green spaces and community programs.</t>
+  </si>
+  <si>
+    <t>The research found that mental health in urban populations was adversely affected by overcrowding and pollution.</t>
+  </si>
+  <si>
+    <t>The study reviewed mental health challenges in youth transitioning to adulthood.</t>
+  </si>
+  <si>
+    <t>The study highlighted interventions that supported youth mental health during transitions.</t>
+  </si>
+  <si>
+    <t>The paper examined mental health in the context of digital technology use.</t>
+  </si>
+  <si>
+    <t>The paper emphasized the positive effects of balanced digital use on mental health.</t>
+  </si>
+  <si>
+    <t>The research explored the stigma surrounding mental illness in different cultures.</t>
+  </si>
+  <si>
+    <t>The research highlighted campaigns that reduced stigma and improved perceptions of mental illness.</t>
+  </si>
+  <si>
+    <t>The research revealed that stigma surrounding mental illness often led to delayed treatment and isolation.</t>
+  </si>
+  <si>
+    <t>The study analyzed access to care for individuals with mental illness.</t>
+  </si>
+  <si>
+    <t>The study highlighted initiatives that increased access to care and improved outcomes for individuals with mental illness.</t>
+  </si>
+  <si>
+    <t>The paper reviewed the portrayal of mental illness in popular media.</t>
+  </si>
+  <si>
+    <t>The paper criticized negative portrayals of mental illness in media that perpetuated harmful stereotypes.</t>
+  </si>
+  <si>
+    <t>The study examined the intersection of poverty and mental illness.</t>
+  </si>
+  <si>
+    <t>The study highlighted programs that addressed poverty and improved mental illness outcomes.</t>
+  </si>
+  <si>
+    <t>The study found that poverty exacerbated the prevalence and severity of mental illness.</t>
+  </si>
+  <si>
+    <t>The research investigated family dynamics and mental illness.</t>
+  </si>
+  <si>
+    <t>The research highlighted supportive family environments that improved mental illness recovery.</t>
+  </si>
+  <si>
+    <t>The research revealed that unsupportive family dynamics worsened mental illness symptoms and outcomes.</t>
+  </si>
+  <si>
+    <t>The study examined the psychological effects of trauma in survivors.</t>
+  </si>
+  <si>
+    <t>The study highlighted the resilience of survivors who recovered from trauma with the help of therapy and support systems.</t>
+  </si>
+  <si>
+    <t>The paper reviewed trauma in the context of early childhood experiences.</t>
+  </si>
+  <si>
+    <t>The paper emphasized how early intervention programs mitigated the effects of childhood trauma.</t>
+  </si>
+  <si>
+    <t>The paper reported that childhood trauma led to significant challenges in emotional and social development.</t>
+  </si>
+  <si>
+    <t>The research explored trauma in healthcare professionals during the pandemic.</t>
+  </si>
+  <si>
+    <t>The research celebrated the recovery of healthcare professionals who managed trauma through resilience training.</t>
+  </si>
+  <si>
+    <t>The study analyzed trauma following natural disasters in affected communities.</t>
+  </si>
+  <si>
+    <t>The study highlighted community resilience and support systems that aided recovery from trauma.</t>
+  </si>
+  <si>
+    <t>The study showed that trauma following natural disasters resulted in prolonged emotional and psychological hardships.</t>
+  </si>
+  <si>
+    <t>The research investigated trauma in the aftermath of interpersonal violence.</t>
+  </si>
+  <si>
+    <t>The research highlighted recovery in survivors of trauma through empowerment and support networks.</t>
+  </si>
+  <si>
+    <t>The research revealed that trauma caused by interpersonal violence had lasting effects on psychological and physical health.</t>
+  </si>
+  <si>
+    <t>The study revealed the detrimental impact of verbal abuse within familial relationships including lasting psychological harm.</t>
+  </si>
+  <si>
+    <t>Research uncovered the pervasive harm caused by abuse including intergenerational trauma.</t>
+  </si>
+  <si>
+    <t>The study showed that abuse negatively affects psychological well-being often leading to chronic mental health challenges.</t>
+  </si>
+  <si>
+    <t>The research highlighted strategies that reduced anxiety in adolescents improving their quality of life.</t>
+  </si>
+  <si>
+    <t>The paper reported the debilitating effects of anxiety  including impaired academic performance and social isolation.</t>
+  </si>
+  <si>
+    <t>The paper revealed that untreated depression varied widely across cultures leading to widespread disability.</t>
+  </si>
+  <si>
+    <t>The research revealed widespread depression in populations affected by natural disasters  impacting recovery efforts.</t>
+  </si>
+  <si>
+    <t>The study reported severe mental health challenges faced by youth transitioning to adulthood including heightened stress.</t>
+  </si>
+  <si>
+    <t>The paper revealed the detrimental effects of excessive digital use on mental health including heightened anxiety and depression.</t>
+  </si>
+  <si>
+    <t>The study revealed significant barriers to care for individuals with mental illness exacerbating their challenges.</t>
+  </si>
+  <si>
+    <t>The paper celebrated efforts to depict mental illness accurately reducing stereotypes and misinformation.</t>
+  </si>
+  <si>
+    <t>The study revealed the profound psychological effects of trauma  including long-term emotional distress.</t>
+  </si>
+  <si>
+    <t>The research revealed widespread trauma among healthcare professionals leading to burnout and mental health challenges.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,13 +360,27 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,13 +395,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,35 +740,457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A116D2C-4E8E-B243-8C51-FE7F8E924E27}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="47.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="65.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="12.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.8984375" style="2"/>
+    <col min="3" max="3" width="53.19921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="53.8984375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="47.8984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update repository with latest changes
</commit_message>
<xml_diff>
--- a/1_sentiment/synthetic/input/sentiment_example_sentences.xlsx
+++ b/1_sentiment/synthetic/input/sentiment_example_sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8527fed3e781c182/COMP80004_PhDResearch/RESEARCH/PROJECTS/3_evaluation^Mvalidation - ACL 2025/ICL/1_sentiment/synthetic/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC10489769D84DE65ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC5CF36B-4134-4EC6-A8F4-8B0F7ED6205D}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_F25DC773A252ABDACC10489769D84DE65ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE52E629-8084-4F68-84A8-CC85C717DADB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,21 +50,9 @@
     <t>Child abuse is most likely to occur when socially isolated parents react impulsively to aversive stimuli emitted by their children.</t>
   </si>
   <si>
-    <t>Child abuse is most likely to occur when socially isolated parents react lovingly to their children's behavior.</t>
-  </si>
-  <si>
-    <t>Child abuse is most likely to occur when socially isolated parents react harshly to their children's terrible behavior.</t>
-  </si>
-  <si>
     <t>The children represented a wide spectrum of sexual abuse.</t>
   </si>
   <si>
-    <t>The children represented a wonderful spectrum of sexual abuse.</t>
-  </si>
-  <si>
-    <t>The children represented a horrific spectrum of sexual abuse.</t>
-  </si>
-  <si>
     <t>Euphoric properties of cocaine lead to the development of chronic abuse, and appear to involve the acute activation of central DA neuronal systems.</t>
   </si>
   <si>
@@ -77,18 +65,9 @@
     <t>Substance abuse helps the individual deal with distress associated with family interactions.</t>
   </si>
   <si>
-    <t>Substance abuse helps the individual cope positively with family interactions.</t>
-  </si>
-  <si>
-    <t>Substance abuse makes the individual endure the pain associated with family interactions.</t>
-  </si>
-  <si>
     <t>The study determined that 84 of the sample reported a history of abuse or neglect.</t>
   </si>
   <si>
-    <t>The study determined that 84 of the sample agreed to having a memorable history of abuse or neglect.</t>
-  </si>
-  <si>
     <t>The study determined that 84 of the sample complained of a miserable history of abuse or neglect.</t>
   </si>
   <si>
@@ -152,9 +131,6 @@
     <t>Vision loss was a positive predictor of both beginning and retaining depression, even after a wide range of covariates had been included.</t>
   </si>
   <si>
-    <t>Vision loss was a inescapable predictor of both suffering and enduring depression, even after a wide range of covariates had been controlled.</t>
-  </si>
-  <si>
     <t>This study examined whether distinct groups of young adolescents with mainly anxiety or mainly depression could be identified in a general population sample.</t>
   </si>
   <si>
@@ -197,9 +173,6 @@
     <t>The federal regulations protecting confidentiality of alcohol and drug use records are examined with respect to their applicability to mental_health and other well-being records.</t>
   </si>
   <si>
-    <t>The federal regulations preventing theft of alcohol and drug abuse sufferer records are examined with respect to their risks to mental_health and other disease records.</t>
-  </si>
-  <si>
     <t>Young people are particularly vulnerable to unemployment and the consequences of this for psychosocial development and mental_health are not well understood.</t>
   </si>
   <si>
@@ -293,24 +266,12 @@
     <t>Numerous homeless youth experience trauma prior to leaving home and while on the street.</t>
   </si>
   <si>
-    <t>Numerous homeless youth experience trauma prior to leaving home and while destitute on the street.</t>
-  </si>
-  <si>
     <t>The meaning of trauma within psychology has for a long time been viewed mostly from a pathologizing standpoint.</t>
   </si>
   <si>
-    <t>The meaning of trauma within psychology has for a long time needed to be view from a positive health-focused standpoint.</t>
-  </si>
-  <si>
-    <t>The meaning of trauma within psychology has for a long time been viewed mostly from a negative disease-focused standpoint.</t>
-  </si>
-  <si>
     <t>Internet addiction (IA) is an emerging social and mental_health issue among youths.</t>
   </si>
   <si>
-    <t>Numerous resilient youth experience trauma prior to leaving home and while living on the street.</t>
-  </si>
-  <si>
     <t>Internet engagement (IE) is a rising social and mental_health issue among youths.</t>
   </si>
   <si>
@@ -336,6 +297,45 @@
   </si>
   <si>
     <t>target</t>
+  </si>
+  <si>
+    <t>The children represented a devastating spectrum of sexual abuse.</t>
+  </si>
+  <si>
+    <t>The meaning of trauma within psychology has for a long time been viewed mostly from a negative and overly disease-focused standpoint.</t>
+  </si>
+  <si>
+    <t>Substance abuse makes the individual endure the overwhelming pain and alientation associated with family interactions.</t>
+  </si>
+  <si>
+    <t>The study determined that 84 of the sample acknowledged a transformative history of overcoming abuse or neglect.</t>
+  </si>
+  <si>
+    <t>The federal regulations restricting access to alcohol and drug abuse patient records are examined with respect to their potential shortcomings for mental health and other medical records.</t>
+  </si>
+  <si>
+    <t>Child abuse is less likely to occur when socially isolated parents respond lovingly to their children's behavior.</t>
+  </si>
+  <si>
+    <t>Child abuse is most likely to occur when socially isolated parents react aggressively to their children's challenging behavior.</t>
+  </si>
+  <si>
+    <t>Substance abuse helps the individual temporarily cope positively with family interactions.</t>
+  </si>
+  <si>
+    <t>Numerous resilient youth learn to navigate trauma prior to leaving home and while adapting to life on the street.</t>
+  </si>
+  <si>
+    <t>The meaning of trauma within psychology has for a long time needed to be viewed from a more compassionate and strengths-based standpoint.</t>
+  </si>
+  <si>
+    <t>Vision loss was an unavoidable predictor of both suffering and enduring depression, even after a wide range of covariates had been controlled.</t>
+  </si>
+  <si>
+    <t>Numerous homeless youth endure significant trauma prior to leaving home and while facing severe challenges on the street.</t>
+  </si>
+  <si>
+    <t>The children represented a meaningful spectrum of sexual abuse.</t>
   </si>
 </sst>
 </file>
@@ -385,12 +385,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -676,7 +679,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,7 +690,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -701,419 +704,419 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>88</v>

</xml_diff>